<commit_message>
New measurements (single and multiple objects)
</commit_message>
<xml_diff>
--- a/Hardware info.xlsx
+++ b/Hardware info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nordic_projects\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107CD71F-3B68-4746-95C3-A5509D0D3540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C34A6C-0E92-4328-AEDB-CD1B041BA365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>A1</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>black</t>
+  </si>
+  <si>
+    <t>***broke/burnt</t>
   </si>
 </sst>
 </file>
@@ -261,18 +264,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -557,7 +558,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -694,16 +695,16 @@
       <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
         <v>32</v>
       </c>
       <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8">
         <v>683444943</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" t="s">
         <v>35</v>
       </c>
     </row>
@@ -723,28 +724,30 @@
       <c r="E9">
         <v>683652108</v>
       </c>
+      <c r="G9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="17" spans="3:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="18" spans="3:5" x14ac:dyDescent="0.45">
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="9"/>
+      <c r="D18" s="8"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="4"/>
+      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <v>683444943</v>
       </c>
     </row>
@@ -752,34 +755,34 @@
       <c r="C21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="E22" s="3"/>
     </row>
     <row r="23" spans="3:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="7"/>
+      <c r="E23" s="6"/>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.45">
       <c r="C25" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25">
         <v>683156255</v>
       </c>
     </row>

</xml_diff>